<commit_message>
change 12:00 to noon
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-With-Jurisdictions-EW.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-With-Jurisdictions-EW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BC9C12-27FC-E14C-AA3A-4ABC366E6EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1A3D8E-D840-C349-AEDE-614CBCC63CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="436">
   <si>
     <t>First Name</t>
   </si>
@@ -1313,6 +1313,21 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>Noon</t>
+  </si>
+  <si>
+    <t>Midnight</t>
+  </si>
+  <si>
+    <t>00:00</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>03:00</t>
   </si>
 </sst>
 </file>
@@ -2276,7 +2291,7 @@
       <c r="AV2" t="s">
         <v>104</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AW2" s="1" t="s">
         <v>94</v>
       </c>
       <c r="AX2" t="s">
@@ -2593,7 +2608,7 @@
       <c r="AV3" t="s">
         <v>104</v>
       </c>
-      <c r="AW3" t="s">
+      <c r="AW3" s="1" t="s">
         <v>357</v>
       </c>
       <c r="AX3" t="s">
@@ -2907,7 +2922,7 @@
       <c r="AV4" t="s">
         <v>104</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="AW4" s="1" t="s">
         <v>94</v>
       </c>
       <c r="AX4" t="s">
@@ -3212,7 +3227,7 @@
       <c r="AV5" t="s">
         <v>104</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AW5" s="1" t="s">
         <v>358</v>
       </c>
       <c r="AX5" t="s">
@@ -3436,7 +3451,7 @@
       <c r="AV6" t="s">
         <v>104</v>
       </c>
-      <c r="AW6" t="s">
+      <c r="AW6" s="1" t="s">
         <v>94</v>
       </c>
       <c r="AX6" t="s">
@@ -3696,7 +3711,7 @@
       <c r="AV7" t="s">
         <v>158</v>
       </c>
-      <c r="AW7" t="s">
+      <c r="AW7" s="1" t="s">
         <v>359</v>
       </c>
       <c r="AX7" t="s">
@@ -3989,8 +4004,8 @@
       <c r="AV8" t="s">
         <v>104</v>
       </c>
-      <c r="AW8" t="s">
-        <v>94</v>
+      <c r="AW8" s="1" t="s">
+        <v>431</v>
       </c>
       <c r="AX8" t="s">
         <v>232</v>
@@ -4249,8 +4264,8 @@
       <c r="AV9" t="s">
         <v>103</v>
       </c>
-      <c r="AW9" t="s">
-        <v>94</v>
+      <c r="AW9" s="1" t="s">
+        <v>432</v>
       </c>
       <c r="AX9" t="s">
         <v>248</v>
@@ -4528,8 +4543,8 @@
       <c r="AV10" t="s">
         <v>104</v>
       </c>
-      <c r="AW10" t="s">
-        <v>94</v>
+      <c r="AW10" s="1" t="s">
+        <v>433</v>
       </c>
       <c r="AX10" t="s">
         <v>268</v>
@@ -4779,8 +4794,8 @@
       <c r="AV11" t="s">
         <v>104</v>
       </c>
-      <c r="AW11" t="s">
-        <v>94</v>
+      <c r="AW11" s="1" t="s">
+        <v>434</v>
       </c>
       <c r="AX11" t="s">
         <v>284</v>
@@ -5005,6 +5020,9 @@
       </c>
       <c r="AV12" t="s">
         <v>104</v>
+      </c>
+      <c r="AW12" s="1" t="s">
+        <v>435</v>
       </c>
       <c r="BO12" t="s">
         <v>112</v>

</xml_diff>

<commit_message>
SARAALERT-513: Address UAT feedback for custom preferred contact time (#1051)
* address UAT feedback for preferred contact time

* change 12:00 to noon
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-With-Jurisdictions-EW.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-With-Jurisdictions-EW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BC9C12-27FC-E14C-AA3A-4ABC366E6EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1A3D8E-D840-C349-AEDE-614CBCC63CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="436">
   <si>
     <t>First Name</t>
   </si>
@@ -1313,6 +1313,21 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>Noon</t>
+  </si>
+  <si>
+    <t>Midnight</t>
+  </si>
+  <si>
+    <t>00:00</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>03:00</t>
   </si>
 </sst>
 </file>
@@ -2276,7 +2291,7 @@
       <c r="AV2" t="s">
         <v>104</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AW2" s="1" t="s">
         <v>94</v>
       </c>
       <c r="AX2" t="s">
@@ -2593,7 +2608,7 @@
       <c r="AV3" t="s">
         <v>104</v>
       </c>
-      <c r="AW3" t="s">
+      <c r="AW3" s="1" t="s">
         <v>357</v>
       </c>
       <c r="AX3" t="s">
@@ -2907,7 +2922,7 @@
       <c r="AV4" t="s">
         <v>104</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="AW4" s="1" t="s">
         <v>94</v>
       </c>
       <c r="AX4" t="s">
@@ -3212,7 +3227,7 @@
       <c r="AV5" t="s">
         <v>104</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AW5" s="1" t="s">
         <v>358</v>
       </c>
       <c r="AX5" t="s">
@@ -3436,7 +3451,7 @@
       <c r="AV6" t="s">
         <v>104</v>
       </c>
-      <c r="AW6" t="s">
+      <c r="AW6" s="1" t="s">
         <v>94</v>
       </c>
       <c r="AX6" t="s">
@@ -3696,7 +3711,7 @@
       <c r="AV7" t="s">
         <v>158</v>
       </c>
-      <c r="AW7" t="s">
+      <c r="AW7" s="1" t="s">
         <v>359</v>
       </c>
       <c r="AX7" t="s">
@@ -3989,8 +4004,8 @@
       <c r="AV8" t="s">
         <v>104</v>
       </c>
-      <c r="AW8" t="s">
-        <v>94</v>
+      <c r="AW8" s="1" t="s">
+        <v>431</v>
       </c>
       <c r="AX8" t="s">
         <v>232</v>
@@ -4249,8 +4264,8 @@
       <c r="AV9" t="s">
         <v>103</v>
       </c>
-      <c r="AW9" t="s">
-        <v>94</v>
+      <c r="AW9" s="1" t="s">
+        <v>432</v>
       </c>
       <c r="AX9" t="s">
         <v>248</v>
@@ -4528,8 +4543,8 @@
       <c r="AV10" t="s">
         <v>104</v>
       </c>
-      <c r="AW10" t="s">
-        <v>94</v>
+      <c r="AW10" s="1" t="s">
+        <v>433</v>
       </c>
       <c r="AX10" t="s">
         <v>268</v>
@@ -4779,8 +4794,8 @@
       <c r="AV11" t="s">
         <v>104</v>
       </c>
-      <c r="AW11" t="s">
-        <v>94</v>
+      <c r="AW11" s="1" t="s">
+        <v>434</v>
       </c>
       <c r="AX11" t="s">
         <v>284</v>
@@ -5005,6 +5020,9 @@
       </c>
       <c r="AV12" t="s">
         <v>104</v>
+      </c>
+      <c r="AW12" s="1" t="s">
+        <v>435</v>
       </c>
       <c r="BO12" t="s">
         <v>112</v>

</xml_diff>